<commit_message>
new approach for SERO
</commit_message>
<xml_diff>
--- a/src/class_MICRO/results_template.xlsx
+++ b/src/class_MICRO/results_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28530" windowHeight="16395" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28530" windowHeight="16395"/>
   </bookViews>
   <sheets>
     <sheet name="group size &gt; 1" sheetId="1" r:id="rId1"/>
@@ -60,27 +60,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -399,67 +379,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="8" priority="7">
-      <formula>$B1=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>G1&lt;&gt;F1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
-      <formula>$C1=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
@@ -498,6 +417,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$B1=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>G1&lt;&gt;F1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576 I1:I1048576">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>$C1=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B1=""</formula>
     </cfRule>

</xml_diff>